<commit_message>
Testing the full program
</commit_message>
<xml_diff>
--- a/OutputFiles/NerResults.xlsx
+++ b/OutputFiles/NerResults.xlsx
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E41" t="n">
         <v>3</v>
@@ -1564,7 +1564,7 @@
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E42" t="n">
         <v>3</v>
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E49" t="n">
         <v>3</v>
@@ -1780,7 +1780,7 @@
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>45078</v>
+        <v>45292</v>
       </c>
       <c r="E62" t="n">
         <v>4</v>
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>45292</v>
+        <v>45078</v>
       </c>
       <c r="E64" t="n">
         <v>4</v>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="D139" s="2" t="n">
-        <v>46388</v>
+        <v>44927</v>
       </c>
       <c r="E139" t="n">
         <v>6</v>
@@ -4210,7 +4210,7 @@
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>44927</v>
+        <v>46388</v>
       </c>
       <c r="E140" t="n">
         <v>6</v>
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="D166" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E166" t="n">
         <v>7</v>
@@ -4939,7 +4939,7 @@
         </is>
       </c>
       <c r="D167" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E167" t="n">
         <v>7</v>
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="D168" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E168" t="n">
         <v>7</v>
@@ -4993,7 +4993,7 @@
         </is>
       </c>
       <c r="D169" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E169" t="n">
         <v>7</v>
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="D170" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E170" t="n">
         <v>7</v>
@@ -5047,7 +5047,7 @@
         </is>
       </c>
       <c r="D171" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E171" t="n">
         <v>7</v>
@@ -5263,7 +5263,7 @@
         </is>
       </c>
       <c r="D179" s="2" t="n">
-        <v>46023</v>
+        <v>45292</v>
       </c>
       <c r="E179" t="n">
         <v>8</v>
@@ -5290,7 +5290,7 @@
         </is>
       </c>
       <c r="D180" s="2" t="n">
-        <v>45292</v>
+        <v>46023</v>
       </c>
       <c r="E180" t="n">
         <v>8</v>
@@ -5884,7 +5884,7 @@
         </is>
       </c>
       <c r="D202" s="2" t="n">
-        <v>47484</v>
+        <v>54789</v>
       </c>
       <c r="E202" t="n">
         <v>8</v>
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="D204" s="2" t="n">
-        <v>54789</v>
+        <v>47484</v>
       </c>
       <c r="E204" t="n">
         <v>8</v>
@@ -6100,7 +6100,7 @@
         </is>
       </c>
       <c r="D210" s="2" t="n">
-        <v>45261</v>
+        <v>45139</v>
       </c>
       <c r="E210" t="n">
         <v>8</v>
@@ -6127,7 +6127,7 @@
         </is>
       </c>
       <c r="D211" s="2" t="n">
-        <v>45139</v>
+        <v>45261</v>
       </c>
       <c r="E211" t="n">
         <v>8</v>
@@ -6640,7 +6640,7 @@
         </is>
       </c>
       <c r="D230" s="2" t="n">
-        <v>47484</v>
+        <v>54789</v>
       </c>
       <c r="E230" t="n">
         <v>8</v>
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D231" s="2" t="n">
-        <v>54789</v>
+        <v>47484</v>
       </c>
       <c r="E231" t="n">
         <v>8</v>
@@ -6721,7 +6721,7 @@
         </is>
       </c>
       <c r="D233" s="2" t="n">
-        <v>45658</v>
+        <v>44927</v>
       </c>
       <c r="E233" t="n">
         <v>8</v>
@@ -6748,7 +6748,7 @@
         </is>
       </c>
       <c r="D234" s="2" t="n">
-        <v>44927</v>
+        <v>45658</v>
       </c>
       <c r="E234" t="n">
         <v>8</v>
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="D285" s="2" t="n">
-        <v>45658</v>
+        <v>44927</v>
       </c>
       <c r="E285" t="n">
         <v>12</v>
@@ -8152,7 +8152,7 @@
         </is>
       </c>
       <c r="D286" s="2" t="n">
-        <v>44927</v>
+        <v>45658</v>
       </c>
       <c r="E286" t="n">
         <v>12</v>
@@ -8449,7 +8449,7 @@
         </is>
       </c>
       <c r="D297" s="2" t="n">
-        <v>46023</v>
+        <v>45658</v>
       </c>
       <c r="E297" t="n">
         <v>12</v>
@@ -8476,7 +8476,7 @@
         </is>
       </c>
       <c r="D298" s="2" t="n">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="E298" t="n">
         <v>12</v>
@@ -8719,7 +8719,7 @@
         </is>
       </c>
       <c r="D307" s="2" t="n">
-        <v>45047</v>
+        <v>45139</v>
       </c>
       <c r="E307" t="n">
         <v>14</v>
@@ -8746,7 +8746,7 @@
         </is>
       </c>
       <c r="D308" s="2" t="n">
-        <v>45139</v>
+        <v>45047</v>
       </c>
       <c r="E308" t="n">
         <v>14</v>
@@ -10123,7 +10123,7 @@
         </is>
       </c>
       <c r="D359" s="2" t="n">
-        <v>118706</v>
+        <v>45658</v>
       </c>
       <c r="E359" t="n">
         <v>16</v>
@@ -10150,7 +10150,7 @@
         </is>
       </c>
       <c r="D360" s="2" t="n">
-        <v>45658</v>
+        <v>118706</v>
       </c>
       <c r="E360" t="n">
         <v>16</v>
@@ -10501,7 +10501,7 @@
         </is>
       </c>
       <c r="D373" s="2" t="n">
-        <v>47484</v>
+        <v>54789</v>
       </c>
       <c r="E373" t="n">
         <v>19</v>
@@ -10528,7 +10528,7 @@
         </is>
       </c>
       <c r="D374" s="2" t="n">
-        <v>54789</v>
+        <v>47484</v>
       </c>
       <c r="E374" t="n">
         <v>19</v>
@@ -11905,7 +11905,7 @@
         </is>
       </c>
       <c r="D425" s="2" t="n">
-        <v>46023</v>
+        <v>45292</v>
       </c>
       <c r="E425" t="n">
         <v>23</v>
@@ -11932,7 +11932,7 @@
         </is>
       </c>
       <c r="D426" s="2" t="n">
-        <v>45292</v>
+        <v>46023</v>
       </c>
       <c r="E426" t="n">
         <v>23</v>
@@ -12202,7 +12202,7 @@
         </is>
       </c>
       <c r="D436" s="2" t="n">
-        <v>47484</v>
+        <v>45658</v>
       </c>
       <c r="E436" t="n">
         <v>23</v>
@@ -12229,7 +12229,7 @@
         </is>
       </c>
       <c r="D437" s="2" t="n">
-        <v>45658</v>
+        <v>47484</v>
       </c>
       <c r="E437" t="n">
         <v>23</v>
@@ -12499,7 +12499,7 @@
         </is>
       </c>
       <c r="D447" s="2" t="n">
-        <v>45078</v>
+        <v>45505</v>
       </c>
       <c r="E447" t="n">
         <v>24</v>
@@ -12526,7 +12526,7 @@
         </is>
       </c>
       <c r="D448" s="2" t="n">
-        <v>45505</v>
+        <v>45078</v>
       </c>
       <c r="E448" t="n">
         <v>24</v>
@@ -13147,7 +13147,7 @@
         </is>
       </c>
       <c r="D471" s="2" t="n">
-        <v>47484</v>
+        <v>45292</v>
       </c>
       <c r="E471" t="n">
         <v>25</v>
@@ -13174,7 +13174,7 @@
         </is>
       </c>
       <c r="D472" s="2" t="n">
-        <v>45292</v>
+        <v>47484</v>
       </c>
       <c r="E472" t="n">
         <v>25</v>
@@ -13876,7 +13876,7 @@
         </is>
       </c>
       <c r="D498" s="2" t="n">
-        <v>47484</v>
+        <v>51136</v>
       </c>
       <c r="E498" t="n">
         <v>28</v>
@@ -13903,7 +13903,7 @@
         </is>
       </c>
       <c r="D499" s="2" t="n">
-        <v>51136</v>
+        <v>47484</v>
       </c>
       <c r="E499" t="n">
         <v>28</v>
@@ -13930,7 +13930,7 @@
         </is>
       </c>
       <c r="D500" s="2" t="n">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="E500" t="n">
         <v>28</v>
@@ -13957,7 +13957,7 @@
         </is>
       </c>
       <c r="D501" s="2" t="n">
-        <v>45292</v>
+        <v>45261</v>
       </c>
       <c r="E501" t="n">
         <v>28</v>

</xml_diff>